<commit_message>
update enterprise online banking and quick payment support bank list
</commit_message>
<xml_diff>
--- a/收款类产品支持银行及限额表/网银收款/企业网银支持银行列表.xlsx
+++ b/收款类产品支持银行及限额表/网银收款/企业网银支持银行列表.xlsx
@@ -197,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -205,20 +205,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -502,13 +518,14 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.25" customWidth="1"/>
-    <col min="2" max="2" width="11.75" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.75" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -520,146 +537,146 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>